<commit_message>
Enhance Histogram and Map classes with color mapping for labels and regions; improve layout options and xtick label handling
</commit_message>
<xml_diff>
--- a/ISCO-08.xlsx
+++ b/ISCO-08.xlsx
@@ -17350,12 +17350,6 @@
 
 <file path=xl/revisions/revisionHeaders.xml><?xml version="1.0" encoding="utf-8"?>
 <headers xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac" guid="{4C7CE3BA-20FA-4653-8613-0C1F352FDCD2}" diskRevisions="1" revisionId="2587" version="4">
-  <header guid="{B033EB84-6E5E-4C3E-B8A1-17F1D3B123E1}" dateTime="2021-08-02T11:31:31" maxSheetId="3" userName="Badre, Lara" r:id="rId540" minRId="2586">
-    <sheetIdMap count="2">
-      <sheetId val="1"/>
-      <sheetId val="2"/>
-    </sheetIdMap>
-  </header>
   <header guid="{4C7CE3BA-20FA-4653-8613-0C1F352FDCD2}" dateTime="2021-08-03T10:12:48" maxSheetId="3" userName="Badre, Lara" r:id="rId541" minRId="2587">
     <sheetIdMap count="2">
       <sheetId val="1"/>
@@ -17363,12 +17357,6 @@
     </sheetIdMap>
   </header>
 </headers>
-</file>
-
-<file path=xl/revisions/revisionLog1.xml><?xml version="1.0" encoding="utf-8"?>
-<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <rsnm rId="2586" sheetId="1" oldName="[ISCO-08 EN Structure and definitions.xlsx]Final ISCO-08" newName="[ISCO-08 EN Structure and definitions.xlsx]ISCO-08 EN"/>
-</revisions>
 </file>
 
 <file path=xl/revisions/revisionLog2.xml><?xml version="1.0" encoding="utf-8"?>

</xml_diff>

<commit_message>
Update job sectors classification with hierarchical structure and improve formatting
</commit_message>
<xml_diff>
--- a/ISCO-08.xlsx
+++ b/ISCO-08.xlsx
@@ -17366,7 +17366,9 @@
 </file>
 
 <file path=xl/revisions/userNames.xml><?xml version="1.0" encoding="utf-8"?>
-<users xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac" count="0"/>
+<users xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac" count="1">
+  <userInfo guid="{4C7CE3BA-20FA-4653-8613-0C1F352FDCD2}" name="User" id="-886995103" dateTime="2025-03-20T11:53:15"/>
+</users>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>

</xml_diff>